<commit_message>
+ work tracking for admin;  * fixed bugs
</commit_message>
<xml_diff>
--- a/ItemsToImport 2.xlsx
+++ b/ItemsToImport 2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Tên món</t>
   </si>
@@ -40,10 +40,43 @@
     <t>Cà phê sữa</t>
   </si>
   <si>
-    <t>Thuốc lá ngoại</t>
-  </si>
-  <si>
-    <t>Mắm ruốc</t>
+    <t>Cà phê đen</t>
+  </si>
+  <si>
+    <t>Thuốc White Horse</t>
+  </si>
+  <si>
+    <t>Nước cam</t>
+  </si>
+  <si>
+    <t>Chanh dây</t>
+  </si>
+  <si>
+    <t>Coca Cola</t>
+  </si>
+  <si>
+    <t>Number One</t>
+  </si>
+  <si>
+    <t>Bò húc</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>Nutriboost</t>
+  </si>
+  <si>
+    <t>Nước dừa</t>
+  </si>
+  <si>
+    <t>Trái</t>
+  </si>
+  <si>
+    <t>Lemoncello</t>
+  </si>
+  <si>
+    <t>Shot</t>
   </si>
 </sst>
 </file>
@@ -385,16 +418,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.875" customWidth="1"/>
-    <col min="2" max="2" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -422,7 +455,7 @@
         <v>8000</v>
       </c>
       <c r="D2">
-        <v>20000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -430,13 +463,13 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>30000</v>
+        <v>7000</v>
       </c>
       <c r="D3">
-        <v>29000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -444,13 +477,125 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>20000</v>
+      </c>
+      <c r="D4">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5000</v>
+      </c>
+      <c r="D5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>12000</v>
+      </c>
+      <c r="D6">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>21000</v>
-      </c>
-      <c r="D4">
-        <v>34000</v>
+      <c r="C7">
+        <v>3000</v>
+      </c>
+      <c r="D7">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>7000</v>
+      </c>
+      <c r="D8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>12000</v>
+      </c>
+      <c r="D9">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>12000</v>
+      </c>
+      <c r="D10">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>30000</v>
+      </c>
+      <c r="D11">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>70000</v>
+      </c>
+      <c r="D12">
+        <v>90000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>